<commit_message>
Added schedule and ganttchart
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g6t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4BBE2A-5307-46C4-B0F4-FB1F953323C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEA535F-00D9-4A75-BADD-0596473839B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
   <si>
     <t>Question</t>
   </si>
@@ -110,6 +110,12 @@
   <si>
     <t>NA</t>
   </si>
+  <si>
+    <t>Created remainder of DAO files from what Maurice did on Saturday, added deleteAll and add method to all DAO files for bootstrap.</t>
+  </si>
+  <si>
+    <t>Created Login page with authentication from database</t>
+  </si>
 </sst>
 </file>
 
@@ -125,18 +131,22 @@
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -213,13 +223,19 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -229,14 +245,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,9 +533,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <selection pane="topRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -540,21 +550,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -574,8 +584,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
@@ -616,221 +626,225 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="17"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="17"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -4809,21 +4823,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -4843,8 +4857,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
@@ -4885,7 +4899,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -4898,7 +4912,7 @@
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
@@ -4909,7 +4923,7 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -4920,7 +4934,7 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -4933,7 +4947,7 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -4944,7 +4958,7 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -4955,7 +4969,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -4968,7 +4982,7 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -4979,7 +4993,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -4990,7 +5004,7 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -5003,7 +5017,7 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -5014,7 +5028,7 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -5025,7 +5039,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -5038,7 +5052,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -5049,7 +5063,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Updated DU for 18/09
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g6t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6343AA54-18E7-49C4-947D-ECF3B98C0592}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E87C0D-1378-4704-AC42-FFDC1833DC5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="42">
   <si>
     <t>Question</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>What will you do today?</t>
-  </si>
-  <si>
-    <t>Week: &lt;starting date&gt; to &lt;ending date&gt;</t>
   </si>
   <si>
     <t>Week 4: 9 September 2019 to 15 September 2019</t>
@@ -137,6 +134,23 @@
   <si>
     <t>Problem with data validation for course_completed, prerequisite completed validation</t>
   </si>
+  <si>
+    <t>Week 5: 16 September 2019 to 22 September 2019</t>
+  </si>
+  <si>
+    <t>Meeting to discuss schedule
+Discuss data validation for course_completed and bid table</t>
+  </si>
+  <si>
+    <t>No issues</t>
+  </si>
+  <si>
+    <t>Meeting to discuss schedule
+Discuss data validation for course_completed and bid table</t>
+  </si>
+  <si>
+    <t>No Issues</t>
+  </si>
 </sst>
 </file>
 
@@ -204,7 +218,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +235,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -288,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -347,6 +367,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,7 +680,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -727,7 +750,7 @@
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -752,7 +775,7 @@
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -770,7 +793,7 @@
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
@@ -781,10 +804,10 @@
       <c r="F6" s="9"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>20</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -797,13 +820,13 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>21</v>
-      </c>
       <c r="I7" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -816,18 +839,18 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="I8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -868,7 +891,7 @@
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -878,13 +901,13 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -898,10 +921,10 @@
       <c r="F13" s="9"/>
       <c r="G13" s="13"/>
       <c r="H13" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -916,12 +939,12 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
@@ -946,7 +969,7 @@
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4921,9 +4944,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D17" sqref="D17"/>
+      <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4945,8 +4968,8 @@
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>13</v>
+      <c r="C1" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -5016,18 +5039,20 @@
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
@@ -5037,12 +5062,14 @@
         <v>12</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
@@ -5053,26 +5080,30 @@
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
@@ -5082,12 +5113,14 @@
         <v>8</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
@@ -5098,24 +5131,28 @@
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
@@ -5125,10 +5162,12 @@
         <v>8</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
@@ -5139,24 +5178,28 @@
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
@@ -5166,12 +5209,14 @@
         <v>8</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
@@ -5182,24 +5227,28 @@
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
@@ -5209,12 +5258,14 @@
         <v>8</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
@@ -5225,9 +5276,11 @@
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>

</xml_diff>

<commit_message>
updated DU for 19 september
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g6t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E87C0D-1378-4704-AC42-FFDC1833DC5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AECF24-BF7D-442C-BE2D-E513E14ABA8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="46">
   <si>
     <t>Question</t>
   </si>
@@ -150,6 +150,18 @@
   </si>
   <si>
     <t>No Issues</t>
+  </si>
+  <si>
+    <t>Add new bid, update existing bid functionality with Sujuan</t>
+  </si>
+  <si>
+    <t>Update and debug existing bid functionality with Sujuan</t>
+  </si>
+  <si>
+    <t>Add new bid, update existing bid functionality with Maurice</t>
+  </si>
+  <si>
+    <t>Update and debug existing bid functionality with Maurice</t>
   </si>
 </sst>
 </file>
@@ -308,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -343,6 +355,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -369,7 +384,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -673,21 +688,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -707,8 +722,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
@@ -749,7 +764,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -764,7 +779,7 @@
       <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
@@ -779,7 +794,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -792,7 +807,7 @@
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -811,7 +826,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
@@ -830,7 +845,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
@@ -849,7 +864,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -864,7 +879,7 @@
       <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
@@ -877,7 +892,7 @@
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -890,7 +905,7 @@
       <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -911,7 +926,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -928,7 +943,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -943,7 +958,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -958,7 +973,7 @@
       <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -973,7 +988,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -4944,9 +4959,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F5" sqref="F5"/>
+      <selection pane="topRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4962,21 +4977,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -4996,8 +5011,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
@@ -5038,7 +5053,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5053,11 +5068,13 @@
       <c r="E3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -5070,11 +5087,11 @@
       <c r="E4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -5085,11 +5102,11 @@
       <c r="E5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5104,11 +5121,13 @@
       <c r="E6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -5121,11 +5140,13 @@
       <c r="E7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5134,11 +5155,13 @@
       <c r="E8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5150,14 +5173,16 @@
       <c r="D9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -5168,11 +5193,11 @@
       <c r="E10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -5181,11 +5206,11 @@
       <c r="E11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -5200,11 +5225,13 @@
       <c r="E12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="24" t="s">
+        <v>44</v>
+      </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -5217,11 +5244,13 @@
       <c r="E13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -5230,11 +5259,13 @@
       <c r="E14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -5249,11 +5280,13 @@
       <c r="E15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -5266,11 +5299,11 @@
       <c r="E16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -5281,7 +5314,7 @@
       <c r="E17" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated DU for 20 sept
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g6t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AECF24-BF7D-442C-BE2D-E513E14ABA8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDB206D-4553-4798-A206-EC127D7132D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="46">
   <si>
     <t>Question</t>
   </si>
@@ -168,7 +168,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -182,11 +182,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -320,18 +315,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -340,31 +332,34 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -374,17 +369,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,11 +672,11 @@
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="32" style="6" customWidth="1"/>
-    <col min="5" max="5" width="31" style="6" customWidth="1"/>
-    <col min="6" max="6" width="30.88671875" style="6" customWidth="1"/>
-    <col min="7" max="9" width="29.109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="32" style="5" customWidth="1"/>
+    <col min="5" max="5" width="31" style="5" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" style="5" customWidth="1"/>
+    <col min="7" max="9" width="29.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -724,25 +716,25 @@
     <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="1"/>
@@ -770,26 +762,26 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12" t="s">
         <v>23</v>
       </c>
     </row>
@@ -798,13 +790,13 @@
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
@@ -813,15 +805,15 @@
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -830,17 +822,17 @@
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="13" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -849,17 +841,17 @@
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="13" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -870,39 +862,39 @@
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
@@ -911,17 +903,17 @@
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -930,15 +922,15 @@
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="10" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -947,13 +939,13 @@
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="10" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -964,26 +956,26 @@
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -992,13 +984,13 @@
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -4959,21 +4951,21 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H4" sqref="H4"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="32" style="6" customWidth="1"/>
-    <col min="5" max="5" width="31" style="6" customWidth="1"/>
-    <col min="6" max="6" width="30.88671875" style="6" customWidth="1"/>
-    <col min="7" max="9" width="29.109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="14.44140625" style="8"/>
+    <col min="1" max="1" width="16.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="32" style="5" customWidth="1"/>
+    <col min="5" max="5" width="31" style="5" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" style="5" customWidth="1"/>
+    <col min="7" max="9" width="29.109375" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="14.44140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5013,25 +5005,25 @@
     <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="1"/>
@@ -5059,51 +5051,53 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -5112,53 +5106,57 @@
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="10" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
@@ -5167,47 +5165,49 @@
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="5"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="10" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="5"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
@@ -5216,53 +5216,57 @@
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="10" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
@@ -5271,51 +5275,53 @@
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="5"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="23"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="5"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>

</xml_diff>

<commit_message>
updated DU for 22 september
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="64">
   <si>
     <t>Question</t>
   </si>
@@ -130,10 +130,6 @@
     <t>No issues</t>
   </si>
   <si>
-    <t>Meeting to discuss schedule
-Discuss data validation for course_completed and bid table</t>
-  </si>
-  <si>
     <t>No Issues</t>
   </si>
   <si>
@@ -182,12 +178,50 @@
   <si>
     <t>Team Meeting</t>
   </si>
+  <si>
+    <t>Add data validation for course_completed bootstrap</t>
+  </si>
+  <si>
+    <t>Create testcase for login, add bid and bootstrap</t>
+  </si>
+  <si>
+    <t>Add input and logical vaildation for bid section with Sujuan</t>
+  </si>
+  <si>
+    <t>Add input and logical vaildation for bid section</t>
+  </si>
+  <si>
+    <t>Add data validation for course_completed and create test cases</t>
+  </si>
+  <si>
+    <t>Added data validation for student, course, section and prerequisite for bootstrap. (pp with ZiCan)</t>
+  </si>
+  <si>
+    <t>Round 1 bidding form, session for login, logout with Sebastian</t>
+  </si>
+  <si>
+    <t>Add new bid, update existing bid functionality with Sujuan</t>
+  </si>
+  <si>
+    <t>Update and debug existing bid functionality with Sujuan</t>
+  </si>
+  <si>
+    <t>session for login, logout, added get course by student id. started round 1 bidding form with Sebastian.</t>
+  </si>
+  <si>
+    <t>Filters for sections to bid with Sujuan</t>
+  </si>
+  <si>
+    <t>Meeting to discuss schedule
+Discuss data validation for course_completed and bid table
+Add new bid, update existing bid functionality with Sujuan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -229,12 +263,6 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -340,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -363,19 +391,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -394,17 +416,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,7 +697,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -691,7 +710,7 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G3" sqref="G3:I17"/>
     </sheetView>
@@ -708,21 +727,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -742,8 +761,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="16.5" thickBot="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -784,7 +803,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" thickBot="1">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -798,14 +817,14 @@
         <v>22</v>
       </c>
       <c r="H3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" thickBot="1">
-      <c r="A4" s="18"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
@@ -814,17 +833,17 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A5" s="18"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -836,14 +855,14 @@
         <v>36</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" thickBot="1">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -864,7 +883,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A7" s="18"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
@@ -873,7 +892,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>20</v>
@@ -883,7 +902,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A8" s="18"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
@@ -902,7 +921,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -916,14 +935,14 @@
         <v>22</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A10" s="18"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
@@ -932,17 +951,17 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A11" s="18"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -951,7 +970,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>36</v>
@@ -961,7 +980,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -982,7 +1001,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A13" s="18"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -991,7 +1010,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>26</v>
@@ -1001,7 +1020,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A14" s="18"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1010,7 +1029,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>36</v>
@@ -1020,7 +1039,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1034,14 +1053,14 @@
         <v>22</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A16" s="18"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1050,7 +1069,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>26</v>
@@ -1060,7 +1079,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A17" s="18"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -1069,13 +1088,13 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>36</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15">
@@ -5037,9 +5056,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E7" sqref="E7"/>
+      <selection pane="topRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5055,21 +5074,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -5089,8 +5108,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="16.5" thickBot="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -5131,281 +5150,323 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" thickBot="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" thickBot="1">
-      <c r="A4" s="22"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>27</v>
+        <v>57</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>43</v>
+      <c r="H4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" thickBot="1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>36</v>
+        <v>60</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A7" s="22"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="H7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A8" s="23"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>38</v>
+        <v>30</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>36</v>
+        <v>42</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A10" s="22"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="I10" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A11" s="23"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A13" s="22"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="9" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="12"/>
+        <v>39</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
+      <c r="C14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="E14" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>36</v>
@@ -5413,9 +5474,15 @@
       <c r="G14" s="9" t="s">
         <v>36</v>
       </c>
+      <c r="H14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -5424,7 +5491,7 @@
       <c r="C15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -5433,99 +5500,127 @@
       <c r="F15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A16" s="22"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="G16" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A17" s="23"/>
+      <c r="H16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="63.75" customHeight="1" thickBot="1">
+      <c r="A17" s="21"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" ht="15">
+      <c r="F17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15">
       <c r="A18" s="1"/>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="15">
+    <row r="19" spans="1:9" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="15">
+    <row r="20" spans="1:9" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="15">
+    <row r="21" spans="1:9" ht="15">
       <c r="A21" s="1"/>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="15">
+    <row r="22" spans="1:9" ht="15">
       <c r="A22" s="1"/>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="15">
+    <row r="23" spans="1:9" ht="15">
       <c r="A23" s="1"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="15">
+    <row r="24" spans="1:9" ht="15">
       <c r="A24" s="1"/>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:7" ht="15">
+    <row r="25" spans="1:9" ht="15">
       <c r="A25" s="1"/>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="15">
+    <row r="26" spans="1:9" ht="15">
       <c r="A26" s="1"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="15">
+    <row r="27" spans="1:9" ht="15">
       <c r="A27" s="1"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="15">
+    <row r="28" spans="1:9" ht="15">
       <c r="A28" s="1"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="15">
+    <row r="29" spans="1:9" ht="15">
       <c r="A29" s="1"/>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="15">
+    <row r="30" spans="1:9" ht="15">
       <c r="A30" s="1"/>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="15">
+    <row r="31" spans="1:9" ht="15">
       <c r="A31" s="1"/>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="15">
+    <row r="32" spans="1:9" ht="15">
       <c r="A32" s="1"/>
       <c r="B32" s="4"/>
     </row>

</xml_diff>